<commit_message>
Mar Time sheet added
</commit_message>
<xml_diff>
--- a/Timesheet/Time Sheet Feb-24.xlsx
+++ b/Timesheet/Time Sheet Feb-24.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kumarvse\My-Daily-task-Remainder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9094FD31-36E7-4255-9585-D7250C696950}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{4175448A-E722-490B-BF31-731F29EE110A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="28">
   <si>
     <t>Timesheet for the Month</t>
   </si>
@@ -106,6 +106,9 @@
     <t>ITOC Bangalore</t>
   </si>
   <si>
+    <t>NA</t>
+  </si>
+  <si>
     <t>Present</t>
   </si>
   <si>
@@ -116,9 +119,6 @@
   </si>
   <si>
     <t>09:00Hours</t>
-  </si>
-  <si>
-    <t>Friday</t>
   </si>
 </sst>
 </file>
@@ -1242,7 +1242,7 @@
   <dimension ref="A1:F231"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B1" sqref="A1:XFD1048576"/>
+      <selection activeCell="D5" sqref="D5:F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1263,7 +1263,7 @@
       <c r="D1" s="21"/>
       <c r="E1" s="21"/>
       <c r="F1" s="9">
-        <v>45352</v>
+        <v>45323</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
@@ -1305,7 +1305,7 @@
       </c>
       <c r="C5" s="47"/>
       <c r="D5" s="49">
-        <v>45352</v>
+        <v>45336</v>
       </c>
       <c r="E5" s="49"/>
       <c r="F5" s="49"/>
@@ -1347,10 +1347,10 @@
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="4"/>
       <c r="B9" s="20">
-        <v>45352</v>
+        <v>45323</v>
       </c>
       <c r="C9" s="14">
-        <v>45382</v>
+        <v>45351</v>
       </c>
       <c r="D9" s="22"/>
       <c r="E9" s="22"/>
@@ -1382,21 +1382,17 @@
       </c>
       <c r="B11" s="18">
         <f t="shared" ref="B11:B38" si="0">IF($B$9+A11-1&lt;=$C$9,($B$9+A11-1),"")</f>
-        <v>45352</v>
+        <v>45323</v>
       </c>
       <c r="C11" s="15" t="str">
         <f t="shared" ref="C11:C39" si="1">TEXT(B11,"dddd")</f>
-        <v>Friday</v>
+        <v>Thursday</v>
       </c>
       <c r="D11" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="E11" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="F11" s="22" t="s">
-        <v>26</v>
-      </c>
+      <c r="E11" s="22"/>
+      <c r="F11" s="22"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="17">
@@ -1404,14 +1400,14 @@
       </c>
       <c r="B12" s="18">
         <f t="shared" si="0"/>
-        <v>45353</v>
+        <v>45324</v>
       </c>
       <c r="C12" s="15" t="str">
         <f t="shared" si="1"/>
-        <v>Saturday</v>
+        <v>Friday</v>
       </c>
       <c r="D12" s="22" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E12" s="22"/>
       <c r="F12" s="22"/>
@@ -1422,14 +1418,14 @@
       </c>
       <c r="B13" s="18">
         <f t="shared" si="0"/>
-        <v>45354</v>
+        <v>45325</v>
       </c>
       <c r="C13" s="15" t="str">
         <f t="shared" si="1"/>
-        <v>Sunday</v>
+        <v>Saturday</v>
       </c>
       <c r="D13" s="22" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E13" s="22"/>
       <c r="F13" s="22"/>
@@ -1440,21 +1436,17 @@
       </c>
       <c r="B14" s="18">
         <f t="shared" si="0"/>
-        <v>45355</v>
+        <v>45326</v>
       </c>
       <c r="C14" s="15" t="str">
         <f t="shared" si="1"/>
-        <v>Monday</v>
+        <v>Sunday</v>
       </c>
       <c r="D14" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="E14" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="F14" s="22" t="s">
-        <v>26</v>
-      </c>
+      <c r="E14" s="22"/>
+      <c r="F14" s="22"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" s="17">
@@ -1462,21 +1454,17 @@
       </c>
       <c r="B15" s="18">
         <f t="shared" si="0"/>
-        <v>45356</v>
+        <v>45327</v>
       </c>
       <c r="C15" s="15" t="str">
         <f t="shared" si="1"/>
-        <v>Tuesday</v>
+        <v>Monday</v>
       </c>
       <c r="D15" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="E15" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="F15" s="22" t="s">
-        <v>26</v>
-      </c>
+      <c r="E15" s="22"/>
+      <c r="F15" s="22"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" s="17">
@@ -1484,21 +1472,17 @@
       </c>
       <c r="B16" s="18">
         <f t="shared" si="0"/>
-        <v>45357</v>
+        <v>45328</v>
       </c>
       <c r="C16" s="15" t="str">
         <f t="shared" si="1"/>
-        <v>Wednesday</v>
+        <v>Tuesday</v>
       </c>
       <c r="D16" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="E16" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="F16" s="22" t="s">
-        <v>26</v>
-      </c>
+      <c r="E16" s="22"/>
+      <c r="F16" s="22"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" s="17">
@@ -1506,21 +1490,17 @@
       </c>
       <c r="B17" s="18">
         <f t="shared" si="0"/>
-        <v>45358</v>
+        <v>45329</v>
       </c>
       <c r="C17" s="15" t="str">
         <f t="shared" si="1"/>
-        <v>Thursday</v>
+        <v>Wednesday</v>
       </c>
       <c r="D17" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="E17" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="F17" s="22" t="s">
-        <v>26</v>
-      </c>
+      <c r="E17" s="22"/>
+      <c r="F17" s="22"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" s="17">
@@ -1528,21 +1508,17 @@
       </c>
       <c r="B18" s="18">
         <f t="shared" si="0"/>
-        <v>45359</v>
+        <v>45330</v>
       </c>
       <c r="C18" s="15" t="str">
         <f t="shared" si="1"/>
-        <v>Friday</v>
+        <v>Thursday</v>
       </c>
       <c r="D18" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="E18" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="F18" s="22" t="s">
-        <v>26</v>
-      </c>
+      <c r="E18" s="22"/>
+      <c r="F18" s="22"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" s="17">
@@ -1550,14 +1526,14 @@
       </c>
       <c r="B19" s="18">
         <f t="shared" si="0"/>
-        <v>45360</v>
+        <v>45331</v>
       </c>
       <c r="C19" s="15" t="str">
         <f t="shared" si="1"/>
-        <v>Saturday</v>
+        <v>Friday</v>
       </c>
       <c r="D19" s="22" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E19" s="22"/>
       <c r="F19" s="22"/>
@@ -1568,14 +1544,14 @@
       </c>
       <c r="B20" s="18">
         <f t="shared" si="0"/>
-        <v>45361</v>
+        <v>45332</v>
       </c>
       <c r="C20" s="15" t="str">
         <f t="shared" si="1"/>
-        <v>Sunday</v>
+        <v>Saturday</v>
       </c>
       <c r="D20" s="22" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E20" s="22"/>
       <c r="F20" s="22"/>
@@ -1586,21 +1562,17 @@
       </c>
       <c r="B21" s="18">
         <f t="shared" si="0"/>
-        <v>45362</v>
+        <v>45333</v>
       </c>
       <c r="C21" s="15" t="str">
         <f t="shared" si="1"/>
-        <v>Monday</v>
+        <v>Sunday</v>
       </c>
       <c r="D21" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="E21" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="F21" s="22" t="s">
-        <v>26</v>
-      </c>
+      <c r="E21" s="22"/>
+      <c r="F21" s="22"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" s="17">
@@ -1608,21 +1580,17 @@
       </c>
       <c r="B22" s="18">
         <f t="shared" si="0"/>
-        <v>45363</v>
+        <v>45334</v>
       </c>
       <c r="C22" s="15" t="str">
         <f t="shared" si="1"/>
-        <v>Tuesday</v>
+        <v>Monday</v>
       </c>
       <c r="D22" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="E22" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="F22" s="22" t="s">
-        <v>26</v>
-      </c>
+      <c r="E22" s="22"/>
+      <c r="F22" s="22"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" s="17">
@@ -1630,21 +1598,17 @@
       </c>
       <c r="B23" s="18">
         <f t="shared" si="0"/>
-        <v>45364</v>
+        <v>45335</v>
       </c>
       <c r="C23" s="15" t="str">
         <f t="shared" si="1"/>
-        <v>Wednesday</v>
+        <v>Tuesday</v>
       </c>
       <c r="D23" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="E23" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="F23" s="22" t="s">
-        <v>26</v>
-      </c>
+      <c r="E23" s="22"/>
+      <c r="F23" s="22"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" s="17">
@@ -1652,20 +1616,20 @@
       </c>
       <c r="B24" s="18">
         <f t="shared" si="0"/>
-        <v>45365</v>
+        <v>45336</v>
       </c>
       <c r="C24" s="15" t="str">
         <f t="shared" si="1"/>
-        <v>Thursday</v>
+        <v>Wednesday</v>
       </c>
       <c r="D24" s="22" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E24" s="22" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F24" s="22" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.35">
@@ -1674,20 +1638,20 @@
       </c>
       <c r="B25" s="18">
         <f t="shared" si="0"/>
-        <v>45366</v>
+        <v>45337</v>
       </c>
       <c r="C25" s="15" t="str">
         <f t="shared" si="1"/>
-        <v>Friday</v>
+        <v>Thursday</v>
       </c>
       <c r="D25" s="22" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E25" s="22" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F25" s="22" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.35">
@@ -1696,17 +1660,21 @@
       </c>
       <c r="B26" s="18">
         <f t="shared" si="0"/>
-        <v>45367</v>
+        <v>45338</v>
       </c>
       <c r="C26" s="15" t="str">
         <f t="shared" si="1"/>
-        <v>Saturday</v>
+        <v>Friday</v>
       </c>
       <c r="D26" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="E26" s="22"/>
-      <c r="F26" s="22"/>
+      <c r="E26" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="F26" s="22" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" s="17">
@@ -1714,14 +1682,14 @@
       </c>
       <c r="B27" s="18">
         <f t="shared" si="0"/>
-        <v>45368</v>
+        <v>45339</v>
       </c>
       <c r="C27" s="15" t="str">
         <f t="shared" si="1"/>
-        <v>Sunday</v>
+        <v>Saturday</v>
       </c>
       <c r="D27" s="22" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E27" s="22"/>
       <c r="F27" s="22"/>
@@ -1732,21 +1700,17 @@
       </c>
       <c r="B28" s="18">
         <f t="shared" si="0"/>
-        <v>45369</v>
+        <v>45340</v>
       </c>
       <c r="C28" s="15" t="str">
         <f t="shared" si="1"/>
-        <v>Monday</v>
+        <v>Sunday</v>
       </c>
       <c r="D28" s="22" t="s">
-        <v>23</v>
-      </c>
-      <c r="E28" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="F28" s="22" t="s">
-        <v>26</v>
-      </c>
+      <c r="E28" s="22"/>
+      <c r="F28" s="22"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" s="17">
@@ -1754,20 +1718,20 @@
       </c>
       <c r="B29" s="18">
         <f t="shared" si="0"/>
-        <v>45370</v>
+        <v>45341</v>
       </c>
       <c r="C29" s="15" t="str">
         <f t="shared" si="1"/>
-        <v>Tuesday</v>
+        <v>Monday</v>
       </c>
       <c r="D29" s="22" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E29" s="22" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F29" s="22" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.35">
@@ -1776,20 +1740,20 @@
       </c>
       <c r="B30" s="18">
         <f t="shared" si="0"/>
-        <v>45371</v>
+        <v>45342</v>
       </c>
       <c r="C30" s="15" t="str">
         <f t="shared" si="1"/>
-        <v>Wednesday</v>
+        <v>Tuesday</v>
       </c>
       <c r="D30" s="22" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E30" s="22" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F30" s="22" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.35">
@@ -1799,20 +1763,20 @@
       </c>
       <c r="B31" s="18">
         <f t="shared" si="0"/>
-        <v>45372</v>
+        <v>45343</v>
       </c>
       <c r="C31" s="15" t="str">
         <f t="shared" si="1"/>
-        <v>Thursday</v>
+        <v>Wednesday</v>
       </c>
       <c r="D31" s="22" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E31" s="22" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F31" s="22" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.35">
@@ -1822,20 +1786,20 @@
       </c>
       <c r="B32" s="18">
         <f t="shared" si="0"/>
-        <v>45373</v>
+        <v>45344</v>
       </c>
       <c r="C32" s="15" t="str">
         <f t="shared" si="1"/>
-        <v>Friday</v>
+        <v>Thursday</v>
       </c>
       <c r="D32" s="22" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E32" s="22" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F32" s="22" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.35">
@@ -1845,17 +1809,21 @@
       </c>
       <c r="B33" s="18">
         <f t="shared" si="0"/>
-        <v>45374</v>
+        <v>45345</v>
       </c>
       <c r="C33" s="15" t="str">
         <f t="shared" si="1"/>
-        <v>Saturday</v>
+        <v>Friday</v>
       </c>
       <c r="D33" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="E33" s="22"/>
-      <c r="F33" s="22"/>
+      <c r="E33" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="F33" s="22" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A34" s="17">
@@ -1864,14 +1832,14 @@
       </c>
       <c r="B34" s="18">
         <f t="shared" si="0"/>
-        <v>45375</v>
+        <v>45346</v>
       </c>
       <c r="C34" s="15" t="str">
         <f t="shared" si="1"/>
-        <v>Sunday</v>
+        <v>Saturday</v>
       </c>
       <c r="D34" s="22" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E34" s="22"/>
       <c r="F34" s="22"/>
@@ -1883,21 +1851,17 @@
       </c>
       <c r="B35" s="18">
         <f t="shared" si="0"/>
-        <v>45376</v>
+        <v>45347</v>
       </c>
       <c r="C35" s="15" t="str">
         <f t="shared" si="1"/>
-        <v>Monday</v>
+        <v>Sunday</v>
       </c>
       <c r="D35" s="22" t="s">
-        <v>23</v>
-      </c>
-      <c r="E35" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="F35" s="22" t="s">
-        <v>26</v>
-      </c>
+      <c r="E35" s="22"/>
+      <c r="F35" s="22"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A36" s="17">
@@ -1906,20 +1870,20 @@
       </c>
       <c r="B36" s="18">
         <f t="shared" si="0"/>
-        <v>45377</v>
+        <v>45348</v>
       </c>
       <c r="C36" s="15" t="str">
         <f t="shared" si="1"/>
-        <v>Tuesday</v>
+        <v>Monday</v>
       </c>
       <c r="D36" s="22" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E36" s="22" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F36" s="22" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.35">
@@ -1929,20 +1893,20 @@
       </c>
       <c r="B37" s="18">
         <f t="shared" si="0"/>
-        <v>45378</v>
+        <v>45349</v>
       </c>
       <c r="C37" s="15" t="str">
         <f t="shared" si="1"/>
-        <v>Wednesday</v>
+        <v>Tuesday</v>
       </c>
       <c r="D37" s="22" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E37" s="22" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F37" s="22" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.35">
@@ -1952,20 +1916,20 @@
       </c>
       <c r="B38" s="26">
         <f t="shared" si="0"/>
-        <v>45379</v>
+        <v>45350</v>
       </c>
       <c r="C38" s="24" t="str">
         <f t="shared" si="1"/>
-        <v>Thursday</v>
+        <v>Wednesday</v>
       </c>
       <c r="D38" s="25" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E38" s="22" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F38" s="22" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.35">
@@ -1973,17 +1937,18 @@
       <c r="B39" s="18">
         <v>45351</v>
       </c>
-      <c r="C39" s="15" t="s">
+      <c r="C39" s="15" t="str">
+        <f t="shared" si="1"/>
+        <v>Thursday</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E39" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="F39" s="22" t="s">
         <v>27</v>
-      </c>
-      <c r="D39" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E39" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="F39" s="22" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.35">

</xml_diff>